<commit_message>
Added test for checking error msg when confirmation password is empty
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="UserDataSet" sheetId="1" r:id="rId1"/>
@@ -152,8 +152,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,9 +330,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,6 +382,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -539,14 +575,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
@@ -555,7 +591,7 @@
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -589,7 +625,7 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -606,7 +642,7 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -623,7 +659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -640,7 +676,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -657,7 +693,7 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -674,7 +710,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -691,7 +727,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -708,7 +744,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75">
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -725,7 +761,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -742,7 +778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -759,7 +795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -776,7 +812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -793,7 +829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -810,7 +846,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -848,21 +884,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +911,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -886,7 +922,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -897,7 +933,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -908,7 +944,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -919,7 +955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -928,7 +964,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Add SetUp property, fixies on test and data bind values on excel
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Key</t>
   </si>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,9 +615,7 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="1">
         <v>12345678</v>
       </c>
@@ -629,9 +627,7 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -652,12 +648,8 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -706,9 +698,7 @@
       <c r="D7" s="1">
         <v>4321</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -765,18 +755,12 @@
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1">
         <v>123</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -785,15 +769,9 @@
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -802,15 +780,11 @@
       <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1">
         <v>12345</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -819,15 +793,11 @@
       <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="1">
         <v>123</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -836,15 +806,11 @@
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="1">
         <v>123</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -853,15 +819,11 @@
       <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="1">
         <v>1234</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
-edit, delete operations with users -changes in the data - xlsx file -User structure
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
+++ b/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/UserData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Key</t>
   </si>
@@ -147,13 +147,19 @@
   </si>
   <si>
     <t>LoginUserSuccessfull</t>
+  </si>
+  <si>
+    <t>IsAdmin</t>
+  </si>
+  <si>
+    <t>IsUser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,7 +304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,9 +336,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,6 +371,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -539,14 +547,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
@@ -555,7 +563,7 @@
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,8 +579,14 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -588,8 +602,14 @@
       <c r="E2" s="1">
         <v>12345678</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -605,8 +625,14 @@
       <c r="E3" s="1">
         <v>12345678</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -622,8 +648,14 @@
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -639,8 +671,14 @@
       <c r="E5" s="1">
         <v>12345</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -656,8 +694,14 @@
       <c r="E6" s="1">
         <v>12345678</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -673,8 +717,14 @@
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -690,8 +740,14 @@
       <c r="E8" s="1">
         <v>1234</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -707,8 +763,14 @@
       <c r="E9" s="1">
         <v>123</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75">
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -724,8 +786,14 @@
       <c r="E10" s="1">
         <v>123</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -741,8 +809,14 @@
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -758,8 +832,14 @@
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -775,8 +855,14 @@
       <c r="E13" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -792,8 +878,14 @@
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -809,8 +901,14 @@
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -825,6 +923,12 @@
       </c>
       <c r="E16" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -848,21 +952,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +979,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -886,7 +990,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -897,7 +1001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -908,7 +1012,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -919,7 +1023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -928,7 +1032,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>

</xml_diff>